<commit_message>
2021-04-26 wbs, table명세서 commit
</commit_message>
<xml_diff>
--- a/src/main/document/여신금융협회 대출모집인 WBS.xlsx
+++ b/src/main/document/여신금융협회 대출모집인 WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1CAA2F-B3F3-450C-B029-6E80D87038DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA4D671-EE06-46A9-83BE-F5A43AB83862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="83">
   <si>
     <t>순번</t>
   </si>
@@ -930,6 +930,42 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="distributed"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -957,46 +993,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1026,18 +1065,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="distributed"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="distributed"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="distributed" wrapText="1"/>
     </xf>
@@ -1071,43 +1104,10 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="distributed" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1413,16 +1413,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:131" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="77"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="66"/>
       <c r="J1" s="18"/>
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
@@ -1454,14 +1454,14 @@
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:131" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="78"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="69"/>
       <c r="J2" s="17"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -1495,206 +1495,206 @@
       <c r="AN2" s="2"/>
     </row>
     <row r="3" spans="1:131" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="68"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="70"/>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="70"/>
-      <c r="AG3" s="70"/>
-      <c r="AH3" s="70"/>
-      <c r="AI3" s="70"/>
-      <c r="AJ3" s="70"/>
-      <c r="AK3" s="70"/>
-      <c r="AL3" s="70"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="82"/>
+      <c r="AC3" s="82"/>
+      <c r="AD3" s="82"/>
+      <c r="AE3" s="82"/>
+      <c r="AF3" s="82"/>
+      <c r="AG3" s="82"/>
+      <c r="AH3" s="82"/>
+      <c r="AI3" s="82"/>
+      <c r="AJ3" s="82"/>
+      <c r="AK3" s="82"/>
+      <c r="AL3" s="82"/>
     </row>
     <row r="4" spans="1:131" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="82"/>
-      <c r="G4" s="81" t="s">
+      <c r="F4" s="71"/>
+      <c r="G4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="82"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="73" t="s">
+      <c r="J4" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="74"/>
-      <c r="AE4" s="74"/>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74"/>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="74"/>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="74"/>
-      <c r="AM4" s="74"/>
-      <c r="AN4" s="74"/>
-      <c r="AO4" s="62" t="s">
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="84"/>
+      <c r="V4" s="84"/>
+      <c r="W4" s="84"/>
+      <c r="X4" s="84"/>
+      <c r="Y4" s="84"/>
+      <c r="Z4" s="84"/>
+      <c r="AA4" s="84"/>
+      <c r="AB4" s="84"/>
+      <c r="AC4" s="84"/>
+      <c r="AD4" s="84"/>
+      <c r="AE4" s="84"/>
+      <c r="AF4" s="84"/>
+      <c r="AG4" s="84"/>
+      <c r="AH4" s="84"/>
+      <c r="AI4" s="84"/>
+      <c r="AJ4" s="84"/>
+      <c r="AK4" s="84"/>
+      <c r="AL4" s="84"/>
+      <c r="AM4" s="84"/>
+      <c r="AN4" s="84"/>
+      <c r="AO4" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="AP4" s="63"/>
-      <c r="AQ4" s="63"/>
-      <c r="AR4" s="63"/>
-      <c r="AS4" s="63"/>
-      <c r="AT4" s="63"/>
-      <c r="AU4" s="63"/>
-      <c r="AV4" s="63"/>
-      <c r="AW4" s="63"/>
-      <c r="AX4" s="63"/>
-      <c r="AY4" s="63"/>
-      <c r="AZ4" s="63"/>
-      <c r="BA4" s="63"/>
-      <c r="BB4" s="63"/>
-      <c r="BC4" s="63"/>
-      <c r="BD4" s="63"/>
-      <c r="BE4" s="63"/>
-      <c r="BF4" s="63"/>
-      <c r="BG4" s="63"/>
-      <c r="BH4" s="63"/>
-      <c r="BI4" s="63"/>
-      <c r="BJ4" s="63"/>
-      <c r="BK4" s="63"/>
-      <c r="BL4" s="63"/>
-      <c r="BM4" s="63"/>
-      <c r="BN4" s="63"/>
-      <c r="BO4" s="63"/>
-      <c r="BP4" s="63"/>
-      <c r="BQ4" s="63"/>
-      <c r="BR4" s="63"/>
-      <c r="BS4" s="64" t="s">
+      <c r="AP4" s="75"/>
+      <c r="AQ4" s="75"/>
+      <c r="AR4" s="75"/>
+      <c r="AS4" s="75"/>
+      <c r="AT4" s="75"/>
+      <c r="AU4" s="75"/>
+      <c r="AV4" s="75"/>
+      <c r="AW4" s="75"/>
+      <c r="AX4" s="75"/>
+      <c r="AY4" s="75"/>
+      <c r="AZ4" s="75"/>
+      <c r="BA4" s="75"/>
+      <c r="BB4" s="75"/>
+      <c r="BC4" s="75"/>
+      <c r="BD4" s="75"/>
+      <c r="BE4" s="75"/>
+      <c r="BF4" s="75"/>
+      <c r="BG4" s="75"/>
+      <c r="BH4" s="75"/>
+      <c r="BI4" s="75"/>
+      <c r="BJ4" s="75"/>
+      <c r="BK4" s="75"/>
+      <c r="BL4" s="75"/>
+      <c r="BM4" s="75"/>
+      <c r="BN4" s="75"/>
+      <c r="BO4" s="75"/>
+      <c r="BP4" s="75"/>
+      <c r="BQ4" s="75"/>
+      <c r="BR4" s="75"/>
+      <c r="BS4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="BT4" s="65"/>
-      <c r="BU4" s="65"/>
-      <c r="BV4" s="65"/>
-      <c r="BW4" s="65"/>
-      <c r="BX4" s="65"/>
-      <c r="BY4" s="65"/>
-      <c r="BZ4" s="65"/>
-      <c r="CA4" s="65"/>
-      <c r="CB4" s="65"/>
-      <c r="CC4" s="65"/>
-      <c r="CD4" s="65"/>
-      <c r="CE4" s="65"/>
-      <c r="CF4" s="65"/>
-      <c r="CG4" s="65"/>
-      <c r="CH4" s="65"/>
-      <c r="CI4" s="65"/>
-      <c r="CJ4" s="65"/>
-      <c r="CK4" s="65"/>
-      <c r="CL4" s="65"/>
-      <c r="CM4" s="65"/>
-      <c r="CN4" s="65"/>
-      <c r="CO4" s="65"/>
-      <c r="CP4" s="65"/>
-      <c r="CQ4" s="65"/>
-      <c r="CR4" s="65"/>
-      <c r="CS4" s="65"/>
-      <c r="CT4" s="65"/>
-      <c r="CU4" s="65"/>
-      <c r="CV4" s="65"/>
-      <c r="CW4" s="65"/>
-      <c r="CX4" s="66" t="s">
+      <c r="BT4" s="77"/>
+      <c r="BU4" s="77"/>
+      <c r="BV4" s="77"/>
+      <c r="BW4" s="77"/>
+      <c r="BX4" s="77"/>
+      <c r="BY4" s="77"/>
+      <c r="BZ4" s="77"/>
+      <c r="CA4" s="77"/>
+      <c r="CB4" s="77"/>
+      <c r="CC4" s="77"/>
+      <c r="CD4" s="77"/>
+      <c r="CE4" s="77"/>
+      <c r="CF4" s="77"/>
+      <c r="CG4" s="77"/>
+      <c r="CH4" s="77"/>
+      <c r="CI4" s="77"/>
+      <c r="CJ4" s="77"/>
+      <c r="CK4" s="77"/>
+      <c r="CL4" s="77"/>
+      <c r="CM4" s="77"/>
+      <c r="CN4" s="77"/>
+      <c r="CO4" s="77"/>
+      <c r="CP4" s="77"/>
+      <c r="CQ4" s="77"/>
+      <c r="CR4" s="77"/>
+      <c r="CS4" s="77"/>
+      <c r="CT4" s="77"/>
+      <c r="CU4" s="77"/>
+      <c r="CV4" s="77"/>
+      <c r="CW4" s="77"/>
+      <c r="CX4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="CY4" s="67"/>
-      <c r="CZ4" s="67"/>
-      <c r="DA4" s="67"/>
-      <c r="DB4" s="67"/>
-      <c r="DC4" s="67"/>
-      <c r="DD4" s="67"/>
-      <c r="DE4" s="67"/>
-      <c r="DF4" s="67"/>
-      <c r="DG4" s="67"/>
-      <c r="DH4" s="67"/>
-      <c r="DI4" s="67"/>
-      <c r="DJ4" s="67"/>
-      <c r="DK4" s="67"/>
-      <c r="DL4" s="67"/>
-      <c r="DM4" s="67"/>
-      <c r="DN4" s="67"/>
-      <c r="DO4" s="67"/>
-      <c r="DP4" s="67"/>
-      <c r="DQ4" s="67"/>
-      <c r="DR4" s="67"/>
-      <c r="DS4" s="67"/>
-      <c r="DT4" s="67"/>
-      <c r="DU4" s="67"/>
-      <c r="DV4" s="67"/>
-      <c r="DW4" s="67"/>
-      <c r="DX4" s="67"/>
-      <c r="DY4" s="67"/>
-      <c r="DZ4" s="67"/>
-      <c r="EA4" s="67"/>
+      <c r="CY4" s="79"/>
+      <c r="CZ4" s="79"/>
+      <c r="DA4" s="79"/>
+      <c r="DB4" s="79"/>
+      <c r="DC4" s="79"/>
+      <c r="DD4" s="79"/>
+      <c r="DE4" s="79"/>
+      <c r="DF4" s="79"/>
+      <c r="DG4" s="79"/>
+      <c r="DH4" s="79"/>
+      <c r="DI4" s="79"/>
+      <c r="DJ4" s="79"/>
+      <c r="DK4" s="79"/>
+      <c r="DL4" s="79"/>
+      <c r="DM4" s="79"/>
+      <c r="DN4" s="79"/>
+      <c r="DO4" s="79"/>
+      <c r="DP4" s="79"/>
+      <c r="DQ4" s="79"/>
+      <c r="DR4" s="79"/>
+      <c r="DS4" s="79"/>
+      <c r="DT4" s="79"/>
+      <c r="DU4" s="79"/>
+      <c r="DV4" s="79"/>
+      <c r="DW4" s="79"/>
+      <c r="DX4" s="79"/>
+      <c r="DY4" s="79"/>
+      <c r="DZ4" s="79"/>
+      <c r="EA4" s="79"/>
     </row>
     <row r="5" spans="1:131" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="72"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="84"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="73"/>
       <c r="I5" s="9" t="s">
         <v>1</v>
       </c>
@@ -4115,11 +4115,6 @@
     <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E4:F5"/>
-    <mergeCell ref="G4:H5"/>
     <mergeCell ref="AO4:BR4"/>
     <mergeCell ref="BS4:CW4"/>
     <mergeCell ref="CX4:EA4"/>
@@ -4127,6 +4122,11 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="J4:AN4"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:F5"/>
+    <mergeCell ref="G4:H5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4138,9 +4138,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:EB995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP32" sqref="AP32"/>
+      <selection pane="topRight" activeCell="BF19" sqref="BF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -4157,16 +4157,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:132" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="77"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="66"/>
       <c r="K1" s="18"/>
       <c r="L1" s="19"/>
       <c r="M1" s="19"/>
@@ -4198,14 +4198,14 @@
       <c r="AM1" s="3"/>
     </row>
     <row r="2" spans="1:132" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="78"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="69"/>
       <c r="K2" s="17"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -4239,214 +4239,214 @@
       <c r="AO2" s="2"/>
     </row>
     <row r="3" spans="1:132" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="68"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="70"/>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="70"/>
-      <c r="AG3" s="70"/>
-      <c r="AH3" s="70"/>
-      <c r="AI3" s="70"/>
-      <c r="AJ3" s="70"/>
-      <c r="AK3" s="70"/>
-      <c r="AL3" s="70"/>
-      <c r="AM3" s="70"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="82"/>
+      <c r="AC3" s="82"/>
+      <c r="AD3" s="82"/>
+      <c r="AE3" s="82"/>
+      <c r="AF3" s="82"/>
+      <c r="AG3" s="82"/>
+      <c r="AH3" s="82"/>
+      <c r="AI3" s="82"/>
+      <c r="AJ3" s="82"/>
+      <c r="AK3" s="82"/>
+      <c r="AL3" s="82"/>
+      <c r="AM3" s="82"/>
     </row>
     <row r="4" spans="1:132" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="82"/>
-      <c r="G4" s="81" t="s">
+      <c r="F4" s="71"/>
+      <c r="G4" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="82"/>
+      <c r="H4" s="71"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="93" t="s">
+      <c r="J4" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="74"/>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="74"/>
-      <c r="AE4" s="74"/>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74"/>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="74"/>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="74"/>
-      <c r="AM4" s="74"/>
-      <c r="AN4" s="74"/>
-      <c r="AO4" s="74"/>
-      <c r="AP4" s="62" t="s">
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="84"/>
+      <c r="V4" s="84"/>
+      <c r="W4" s="84"/>
+      <c r="X4" s="84"/>
+      <c r="Y4" s="84"/>
+      <c r="Z4" s="84"/>
+      <c r="AA4" s="84"/>
+      <c r="AB4" s="84"/>
+      <c r="AC4" s="84"/>
+      <c r="AD4" s="84"/>
+      <c r="AE4" s="84"/>
+      <c r="AF4" s="84"/>
+      <c r="AG4" s="84"/>
+      <c r="AH4" s="84"/>
+      <c r="AI4" s="84"/>
+      <c r="AJ4" s="84"/>
+      <c r="AK4" s="84"/>
+      <c r="AL4" s="84"/>
+      <c r="AM4" s="84"/>
+      <c r="AN4" s="84"/>
+      <c r="AO4" s="84"/>
+      <c r="AP4" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="AQ4" s="63"/>
-      <c r="AR4" s="63"/>
-      <c r="AS4" s="63"/>
-      <c r="AT4" s="63"/>
-      <c r="AU4" s="63"/>
-      <c r="AV4" s="63"/>
-      <c r="AW4" s="63"/>
-      <c r="AX4" s="63"/>
-      <c r="AY4" s="63"/>
-      <c r="AZ4" s="63"/>
-      <c r="BA4" s="63"/>
-      <c r="BB4" s="63"/>
-      <c r="BC4" s="63"/>
-      <c r="BD4" s="63"/>
-      <c r="BE4" s="63"/>
-      <c r="BF4" s="63"/>
-      <c r="BG4" s="63"/>
-      <c r="BH4" s="63"/>
-      <c r="BI4" s="63"/>
-      <c r="BJ4" s="63"/>
-      <c r="BK4" s="63"/>
-      <c r="BL4" s="63"/>
-      <c r="BM4" s="63"/>
-      <c r="BN4" s="63"/>
-      <c r="BO4" s="63"/>
-      <c r="BP4" s="63"/>
-      <c r="BQ4" s="63"/>
-      <c r="BR4" s="63"/>
-      <c r="BS4" s="63"/>
-      <c r="BT4" s="64" t="s">
+      <c r="AQ4" s="75"/>
+      <c r="AR4" s="75"/>
+      <c r="AS4" s="75"/>
+      <c r="AT4" s="75"/>
+      <c r="AU4" s="75"/>
+      <c r="AV4" s="75"/>
+      <c r="AW4" s="75"/>
+      <c r="AX4" s="75"/>
+      <c r="AY4" s="75"/>
+      <c r="AZ4" s="75"/>
+      <c r="BA4" s="75"/>
+      <c r="BB4" s="75"/>
+      <c r="BC4" s="75"/>
+      <c r="BD4" s="75"/>
+      <c r="BE4" s="75"/>
+      <c r="BF4" s="75"/>
+      <c r="BG4" s="75"/>
+      <c r="BH4" s="75"/>
+      <c r="BI4" s="75"/>
+      <c r="BJ4" s="75"/>
+      <c r="BK4" s="75"/>
+      <c r="BL4" s="75"/>
+      <c r="BM4" s="75"/>
+      <c r="BN4" s="75"/>
+      <c r="BO4" s="75"/>
+      <c r="BP4" s="75"/>
+      <c r="BQ4" s="75"/>
+      <c r="BR4" s="75"/>
+      <c r="BS4" s="75"/>
+      <c r="BT4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="BU4" s="65"/>
-      <c r="BV4" s="65"/>
-      <c r="BW4" s="65"/>
-      <c r="BX4" s="65"/>
-      <c r="BY4" s="65"/>
-      <c r="BZ4" s="65"/>
-      <c r="CA4" s="65"/>
-      <c r="CB4" s="65"/>
-      <c r="CC4" s="65"/>
-      <c r="CD4" s="65"/>
-      <c r="CE4" s="65"/>
-      <c r="CF4" s="65"/>
-      <c r="CG4" s="65"/>
-      <c r="CH4" s="65"/>
-      <c r="CI4" s="65"/>
-      <c r="CJ4" s="65"/>
-      <c r="CK4" s="65"/>
-      <c r="CL4" s="65"/>
-      <c r="CM4" s="65"/>
-      <c r="CN4" s="65"/>
-      <c r="CO4" s="65"/>
-      <c r="CP4" s="65"/>
-      <c r="CQ4" s="65"/>
-      <c r="CR4" s="65"/>
-      <c r="CS4" s="65"/>
-      <c r="CT4" s="65"/>
-      <c r="CU4" s="65"/>
-      <c r="CV4" s="65"/>
-      <c r="CW4" s="65"/>
-      <c r="CX4" s="65"/>
-      <c r="CY4" s="66" t="s">
+      <c r="BU4" s="77"/>
+      <c r="BV4" s="77"/>
+      <c r="BW4" s="77"/>
+      <c r="BX4" s="77"/>
+      <c r="BY4" s="77"/>
+      <c r="BZ4" s="77"/>
+      <c r="CA4" s="77"/>
+      <c r="CB4" s="77"/>
+      <c r="CC4" s="77"/>
+      <c r="CD4" s="77"/>
+      <c r="CE4" s="77"/>
+      <c r="CF4" s="77"/>
+      <c r="CG4" s="77"/>
+      <c r="CH4" s="77"/>
+      <c r="CI4" s="77"/>
+      <c r="CJ4" s="77"/>
+      <c r="CK4" s="77"/>
+      <c r="CL4" s="77"/>
+      <c r="CM4" s="77"/>
+      <c r="CN4" s="77"/>
+      <c r="CO4" s="77"/>
+      <c r="CP4" s="77"/>
+      <c r="CQ4" s="77"/>
+      <c r="CR4" s="77"/>
+      <c r="CS4" s="77"/>
+      <c r="CT4" s="77"/>
+      <c r="CU4" s="77"/>
+      <c r="CV4" s="77"/>
+      <c r="CW4" s="77"/>
+      <c r="CX4" s="77"/>
+      <c r="CY4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="CZ4" s="67"/>
-      <c r="DA4" s="67"/>
-      <c r="DB4" s="67"/>
-      <c r="DC4" s="67"/>
-      <c r="DD4" s="67"/>
-      <c r="DE4" s="67"/>
-      <c r="DF4" s="67"/>
-      <c r="DG4" s="67"/>
-      <c r="DH4" s="67"/>
-      <c r="DI4" s="67"/>
-      <c r="DJ4" s="67"/>
-      <c r="DK4" s="67"/>
-      <c r="DL4" s="67"/>
-      <c r="DM4" s="67"/>
-      <c r="DN4" s="67"/>
-      <c r="DO4" s="67"/>
-      <c r="DP4" s="67"/>
-      <c r="DQ4" s="67"/>
-      <c r="DR4" s="67"/>
-      <c r="DS4" s="67"/>
-      <c r="DT4" s="67"/>
-      <c r="DU4" s="67"/>
-      <c r="DV4" s="67"/>
-      <c r="DW4" s="67"/>
-      <c r="DX4" s="67"/>
-      <c r="DY4" s="67"/>
-      <c r="DZ4" s="67"/>
-      <c r="EA4" s="67"/>
-      <c r="EB4" s="67"/>
+      <c r="CZ4" s="79"/>
+      <c r="DA4" s="79"/>
+      <c r="DB4" s="79"/>
+      <c r="DC4" s="79"/>
+      <c r="DD4" s="79"/>
+      <c r="DE4" s="79"/>
+      <c r="DF4" s="79"/>
+      <c r="DG4" s="79"/>
+      <c r="DH4" s="79"/>
+      <c r="DI4" s="79"/>
+      <c r="DJ4" s="79"/>
+      <c r="DK4" s="79"/>
+      <c r="DL4" s="79"/>
+      <c r="DM4" s="79"/>
+      <c r="DN4" s="79"/>
+      <c r="DO4" s="79"/>
+      <c r="DP4" s="79"/>
+      <c r="DQ4" s="79"/>
+      <c r="DR4" s="79"/>
+      <c r="DS4" s="79"/>
+      <c r="DT4" s="79"/>
+      <c r="DU4" s="79"/>
+      <c r="DV4" s="79"/>
+      <c r="DW4" s="79"/>
+      <c r="DX4" s="79"/>
+      <c r="DY4" s="79"/>
+      <c r="DZ4" s="79"/>
+      <c r="EA4" s="79"/>
+      <c r="EB4" s="79"/>
     </row>
     <row r="5" spans="1:132" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="72"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
       <c r="D5" s="97"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="84"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="73"/>
       <c r="I5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="94"/>
+      <c r="J5" s="96"/>
       <c r="K5" s="5">
         <v>1</v>
       </c>
@@ -4815,13 +4815,13 @@
       </c>
     </row>
     <row r="6" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="104" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="33">
         <v>1</v>
       </c>
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="112" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="27" t="s">
@@ -4965,11 +4965,11 @@
       <c r="EB6" s="13"/>
     </row>
     <row r="7" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="92"/>
+      <c r="A7" s="105"/>
       <c r="B7" s="33">
         <v>2</v>
       </c>
-      <c r="C7" s="102"/>
+      <c r="C7" s="113"/>
       <c r="D7" s="27" t="s">
         <v>30</v>
       </c>
@@ -5109,11 +5109,11 @@
       <c r="EB7" s="13"/>
     </row>
     <row r="8" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="92"/>
+      <c r="A8" s="105"/>
       <c r="B8" s="33">
         <v>3</v>
       </c>
-      <c r="C8" s="102"/>
+      <c r="C8" s="113"/>
       <c r="D8" s="27" t="s">
         <v>24</v>
       </c>
@@ -5253,9 +5253,9 @@
       <c r="EB8" s="13"/>
     </row>
     <row r="9" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="92"/>
+      <c r="A9" s="105"/>
       <c r="B9" s="42"/>
-      <c r="C9" s="102"/>
+      <c r="C9" s="113"/>
       <c r="D9" s="38" t="s">
         <v>8</v>
       </c>
@@ -5393,9 +5393,9 @@
       <c r="EB9" s="13"/>
     </row>
     <row r="10" spans="1:132" s="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="92"/>
+      <c r="A10" s="105"/>
       <c r="B10" s="49"/>
-      <c r="C10" s="102"/>
+      <c r="C10" s="113"/>
       <c r="D10" s="47" t="s">
         <v>75</v>
       </c>
@@ -5411,7 +5411,7 @@
       <c r="H10" s="50"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -5536,11 +5536,11 @@
       <c r="EB10" s="13"/>
     </row>
     <row r="11" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="92"/>
+      <c r="A11" s="105"/>
       <c r="B11" s="42">
         <v>4</v>
       </c>
-      <c r="C11" s="103"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="38" t="s">
         <v>16</v>
       </c>
@@ -5678,22 +5678,22 @@
       <c r="EB11" s="13"/>
     </row>
     <row r="12" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="92" t="s">
+      <c r="A12" s="105" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="33">
         <v>1</v>
       </c>
-      <c r="C12" s="101" t="s">
+      <c r="C12" s="112" t="s">
         <v>32</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="109" t="s">
+      <c r="E12" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="112" t="s">
+      <c r="F12" s="120" t="s">
         <v>53</v>
       </c>
       <c r="G12" s="30"/>
@@ -5824,16 +5824,16 @@
       <c r="EB12" s="13"/>
     </row>
     <row r="13" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="92"/>
+      <c r="A13" s="105"/>
       <c r="B13" s="33">
         <v>2</v>
       </c>
-      <c r="C13" s="102"/>
+      <c r="C13" s="113"/>
       <c r="D13" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="110"/>
-      <c r="F13" s="112"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="120"/>
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
       <c r="I13" s="9"/>
@@ -5962,16 +5962,16 @@
       <c r="EB13" s="13"/>
     </row>
     <row r="14" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="92"/>
+      <c r="A14" s="105"/>
       <c r="B14" s="33">
         <v>3</v>
       </c>
-      <c r="C14" s="102"/>
+      <c r="C14" s="113"/>
       <c r="D14" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="111"/>
-      <c r="F14" s="113"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="121"/>
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
       <c r="I14" s="9"/>
@@ -6100,18 +6100,18 @@
       <c r="EB14" s="13"/>
     </row>
     <row r="15" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="92"/>
+      <c r="A15" s="105"/>
       <c r="B15" s="33">
         <v>4</v>
       </c>
-      <c r="C15" s="102"/>
+      <c r="C15" s="113"/>
       <c r="D15" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="117" t="s">
+      <c r="E15" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="114" t="s">
+      <c r="F15" s="85" t="s">
         <v>52</v>
       </c>
       <c r="G15" s="30"/>
@@ -6242,16 +6242,16 @@
       <c r="EB15" s="13"/>
     </row>
     <row r="16" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="92"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="33">
         <v>5</v>
       </c>
-      <c r="C16" s="102"/>
+      <c r="C16" s="113"/>
       <c r="D16" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="118"/>
-      <c r="F16" s="115"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="86"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
       <c r="I16" s="9"/>
@@ -6380,16 +6380,16 @@
       <c r="EB16" s="13"/>
     </row>
     <row r="17" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="104"/>
+      <c r="A17" s="115"/>
       <c r="B17" s="33">
         <v>6</v>
       </c>
-      <c r="C17" s="103"/>
+      <c r="C17" s="114"/>
       <c r="D17" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="119"/>
-      <c r="F17" s="116"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="87"/>
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
       <c r="I17" s="9"/>
@@ -6518,13 +6518,13 @@
       <c r="EB17" s="13"/>
     </row>
     <row r="18" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="91" t="s">
+      <c r="A18" s="104" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="95" t="s">
+      <c r="C18" s="107" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="40" t="s">
@@ -6668,11 +6668,11 @@
       <c r="EB18" s="13"/>
     </row>
     <row r="19" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="92"/>
+      <c r="A19" s="105"/>
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="105"/>
+      <c r="C19" s="116"/>
       <c r="D19" s="41" t="s">
         <v>25</v>
       </c>
@@ -6683,7 +6683,7 @@
         <v>68</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H19" s="30"/>
       <c r="I19" s="9"/>
@@ -6747,10 +6747,10 @@
       <c r="BM19" s="6"/>
       <c r="BN19" s="6"/>
       <c r="BO19" s="13"/>
-      <c r="BP19" s="13"/>
+      <c r="BP19" s="36"/>
       <c r="BQ19" s="36"/>
-      <c r="BR19" s="36"/>
-      <c r="BS19" s="36"/>
+      <c r="BR19" s="13"/>
+      <c r="BS19" s="13"/>
       <c r="BT19" s="6"/>
       <c r="BU19" s="6"/>
       <c r="BV19" s="59"/>
@@ -6814,11 +6814,11 @@
       <c r="EB19" s="13"/>
     </row>
     <row r="20" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="92"/>
+      <c r="A20" s="105"/>
       <c r="B20" s="1">
         <v>3</v>
       </c>
-      <c r="C20" s="96"/>
+      <c r="C20" s="108"/>
       <c r="D20" s="41" t="s">
         <v>26</v>
       </c>
@@ -6828,7 +6828,9 @@
       <c r="F20" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="20" t="s">
+        <v>67</v>
+      </c>
       <c r="H20" s="30"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -6890,8 +6892,8 @@
       <c r="BN20" s="6"/>
       <c r="BO20" s="13"/>
       <c r="BP20" s="13"/>
-      <c r="BQ20" s="13"/>
-      <c r="BR20" s="13"/>
+      <c r="BQ20" s="36"/>
+      <c r="BR20" s="36"/>
       <c r="BS20" s="13"/>
       <c r="BT20" s="6"/>
       <c r="BU20" s="6"/>
@@ -6956,20 +6958,20 @@
       <c r="EB20" s="13"/>
     </row>
     <row r="21" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="92"/>
+      <c r="A21" s="105"/>
       <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="106" t="s">
+      <c r="C21" s="117" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="120" t="s">
+      <c r="E21" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="120" t="s">
+      <c r="F21" s="94" t="s">
         <v>74</v>
       </c>
       <c r="G21" s="30"/>
@@ -7100,16 +7102,16 @@
       <c r="EB21" s="13"/>
     </row>
     <row r="22" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="92"/>
+      <c r="A22" s="105"/>
       <c r="B22" s="1">
         <v>2</v>
       </c>
-      <c r="C22" s="107"/>
+      <c r="C22" s="118"/>
       <c r="D22" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="121"/>
-      <c r="F22" s="121"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="95"/>
       <c r="G22" s="28"/>
       <c r="H22" s="30"/>
       <c r="I22" s="9"/>
@@ -7238,16 +7240,16 @@
       <c r="EB22" s="13"/>
     </row>
     <row r="23" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="92"/>
+      <c r="A23" s="105"/>
       <c r="B23" s="1">
         <v>3</v>
       </c>
-      <c r="C23" s="107"/>
+      <c r="C23" s="118"/>
       <c r="D23" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="121"/>
-      <c r="F23" s="121"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
       <c r="G23" s="30"/>
       <c r="H23" s="30"/>
       <c r="I23" s="9"/>
@@ -7376,11 +7378,11 @@
       <c r="EB23" s="13"/>
     </row>
     <row r="24" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="92"/>
+      <c r="A24" s="105"/>
       <c r="B24" s="1">
         <v>4</v>
       </c>
-      <c r="C24" s="108"/>
+      <c r="C24" s="119"/>
       <c r="D24" s="38" t="s">
         <v>22</v>
       </c>
@@ -7518,9 +7520,9 @@
       <c r="EB24" s="13"/>
     </row>
     <row r="25" spans="1:132" s="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="92"/>
+      <c r="A25" s="105"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="95" t="s">
+      <c r="C25" s="107" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="48" t="s">
@@ -7538,7 +7540,7 @@
       <c r="H25" s="30"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -7663,11 +7665,11 @@
       <c r="EB25" s="13"/>
     </row>
     <row r="26" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="104"/>
+      <c r="A26" s="115"/>
       <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="96"/>
+      <c r="C26" s="108"/>
       <c r="D26" s="61" t="s">
         <v>19</v>
       </c>
@@ -7683,7 +7685,7 @@
       <c r="H26" s="30"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -7808,22 +7810,22 @@
       <c r="EB26" s="13"/>
     </row>
     <row r="27" spans="1:132" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="91" t="s">
+      <c r="A27" s="104" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
-      <c r="C27" s="98" t="s">
+      <c r="C27" s="109" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="109" t="s">
+      <c r="E27" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="109" t="s">
+      <c r="F27" s="91" t="s">
         <v>71</v>
       </c>
       <c r="G27" s="21"/>
@@ -7954,16 +7956,16 @@
       <c r="EB27" s="13"/>
     </row>
     <row r="28" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="92"/>
+      <c r="A28" s="105"/>
       <c r="B28" s="1">
         <v>2</v>
       </c>
-      <c r="C28" s="99"/>
+      <c r="C28" s="110"/>
       <c r="D28" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="110"/>
-      <c r="F28" s="110"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
       <c r="G28" s="21"/>
       <c r="H28" s="28"/>
       <c r="I28" s="10"/>
@@ -8092,16 +8094,16 @@
       <c r="EB28" s="13"/>
     </row>
     <row r="29" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="92"/>
+      <c r="A29" s="105"/>
       <c r="B29" s="1">
         <v>3</v>
       </c>
-      <c r="C29" s="99"/>
+      <c r="C29" s="110"/>
       <c r="D29" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="111"/>
-      <c r="F29" s="111"/>
+      <c r="E29" s="93"/>
+      <c r="F29" s="93"/>
       <c r="G29" s="21"/>
       <c r="H29" s="28"/>
       <c r="I29" s="10"/>
@@ -8230,11 +8232,11 @@
       <c r="EB29" s="13"/>
     </row>
     <row r="30" spans="1:132" s="37" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="92"/>
+      <c r="A30" s="105"/>
       <c r="B30" s="1">
         <v>4</v>
       </c>
-      <c r="C30" s="99"/>
+      <c r="C30" s="110"/>
       <c r="D30" s="38" t="s">
         <v>22</v>
       </c>
@@ -8372,11 +8374,11 @@
       <c r="EB30" s="13"/>
     </row>
     <row r="31" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="92"/>
+      <c r="A31" s="105"/>
       <c r="B31" s="1">
         <v>5</v>
       </c>
-      <c r="C31" s="100"/>
+      <c r="C31" s="111"/>
       <c r="D31" s="39" t="s">
         <v>24</v>
       </c>
@@ -8514,11 +8516,11 @@
       <c r="EB31" s="13"/>
     </row>
     <row r="32" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="92"/>
+      <c r="A32" s="105"/>
       <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="C32" s="98" t="s">
+      <c r="C32" s="109" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="27" t="s">
@@ -8658,11 +8660,11 @@
       <c r="EB32" s="13"/>
     </row>
     <row r="33" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="92"/>
+      <c r="A33" s="105"/>
       <c r="B33" s="1">
         <v>2</v>
       </c>
-      <c r="C33" s="99"/>
+      <c r="C33" s="110"/>
       <c r="D33" s="27" t="s">
         <v>23</v>
       </c>
@@ -8800,11 +8802,11 @@
       <c r="EB33" s="13"/>
     </row>
     <row r="34" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="92"/>
+      <c r="A34" s="105"/>
       <c r="B34" s="1">
         <v>3</v>
       </c>
-      <c r="C34" s="100"/>
+      <c r="C34" s="111"/>
       <c r="D34" s="27" t="s">
         <v>22</v>
       </c>
@@ -8942,7 +8944,7 @@
       <c r="EB34" s="13"/>
     </row>
     <row r="35" spans="1:132" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="92"/>
+      <c r="A35" s="105"/>
       <c r="B35" s="1">
         <v>1</v>
       </c>
@@ -9086,11 +9088,11 @@
       <c r="EB35" s="13"/>
     </row>
     <row r="36" spans="1:132" s="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="92"/>
+      <c r="A36" s="105"/>
       <c r="B36" s="1">
         <v>1</v>
       </c>
-      <c r="C36" s="88" t="s">
+      <c r="C36" s="101" t="s">
         <v>78</v>
       </c>
       <c r="D36" s="47" t="s">
@@ -9106,7 +9108,7 @@
       <c r="H36" s="54"/>
       <c r="I36" s="10"/>
       <c r="J36" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K36" s="13"/>
       <c r="L36" s="12"/>
@@ -9232,11 +9234,11 @@
       <c r="EB36" s="13"/>
     </row>
     <row r="37" spans="1:132" s="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="92"/>
+      <c r="A37" s="105"/>
       <c r="B37" s="1">
         <v>2</v>
       </c>
-      <c r="C37" s="89"/>
+      <c r="C37" s="102"/>
       <c r="D37" s="47" t="s">
         <v>19</v>
       </c>
@@ -9250,7 +9252,7 @@
       <c r="H37" s="54"/>
       <c r="I37" s="10"/>
       <c r="J37" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K37" s="13"/>
       <c r="L37" s="12"/>
@@ -9376,11 +9378,11 @@
       <c r="EB37" s="13"/>
     </row>
     <row r="38" spans="1:132" s="45" customFormat="1" ht="31.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="92"/>
+      <c r="A38" s="105"/>
       <c r="B38" s="1">
         <v>3</v>
       </c>
-      <c r="C38" s="89"/>
+      <c r="C38" s="102"/>
       <c r="D38" s="47" t="s">
         <v>81</v>
       </c>
@@ -9394,7 +9396,7 @@
       <c r="H38" s="54"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K38" s="13"/>
       <c r="L38" s="12"/>
@@ -9520,11 +9522,11 @@
       <c r="EB38" s="13"/>
     </row>
     <row r="39" spans="1:132" s="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="92"/>
+      <c r="A39" s="105"/>
       <c r="B39" s="1">
         <v>4</v>
       </c>
-      <c r="C39" s="90"/>
+      <c r="C39" s="103"/>
       <c r="D39" s="47" t="s">
         <v>21</v>
       </c>
@@ -9538,7 +9540,7 @@
       <c r="H39" s="54"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K39" s="13"/>
       <c r="L39" s="12"/>
@@ -9810,7 +9812,7 @@
     <row r="41" spans="1:132" s="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="46"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="85"/>
+      <c r="C41" s="98"/>
       <c r="D41" s="47"/>
       <c r="E41" s="56"/>
       <c r="F41" s="56"/>
@@ -9944,7 +9946,7 @@
     <row r="42" spans="1:132" s="45" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="46"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="86"/>
+      <c r="C42" s="99"/>
       <c r="D42" s="47"/>
       <c r="E42" s="56"/>
       <c r="F42" s="56"/>
@@ -10078,7 +10080,7 @@
     <row r="43" spans="1:132" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="29"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="87"/>
+      <c r="C43" s="100"/>
       <c r="D43" s="47"/>
       <c r="E43" s="52"/>
       <c r="F43" s="52"/>
@@ -11163,24 +11165,6 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="AP4:BS4"/>
-    <mergeCell ref="BT4:CX4"/>
-    <mergeCell ref="CY4:EB4"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B3:AM3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="K4:AO4"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:F5"/>
-    <mergeCell ref="G4:H5"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="C36:C39"/>
     <mergeCell ref="A27:A39"/>
@@ -11197,6 +11181,24 @@
     <mergeCell ref="A12:A17"/>
     <mergeCell ref="C12:C17"/>
     <mergeCell ref="F12:F14"/>
+    <mergeCell ref="AP4:BS4"/>
+    <mergeCell ref="BT4:CX4"/>
+    <mergeCell ref="CY4:EB4"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B3:AM3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="K4:AO4"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:F5"/>
+    <mergeCell ref="G4:H5"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2021-04-27 테이블 명세서 추가 및 wbs수정, table ddl 추가 commit
</commit_message>
<xml_diff>
--- a/src/main/document/여신금융협회 대출모집인 WBS.xlsx
+++ b/src/main/document/여신금융협회 대출모집인 WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA4D671-EE06-46A9-83BE-F5A43AB83862}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FC6DC3-8444-4838-81D6-F33054528232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4138,9 +4138,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:EB995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BF19" sqref="BF19"/>
+      <selection pane="topRight" activeCell="AA34" sqref="AA34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>